<commit_message>
new definitions in diageous
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS_SAND/Data/Template.xlsx
+++ b/Projects/DIAGEOUS_SAND/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="65">
   <si>
     <t>KPI Name</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>6. Lock Box Display</t>
+  </si>
+  <si>
+    <t>OTHER</t>
   </si>
   <si>
     <t>MINIMUM SHELF LOCATION</t>
@@ -552,15 +555,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>444600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>283680</xdr:colOff>
+      <xdr:colOff>310320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>365400</xdr:rowOff>
+      <xdr:rowOff>365040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -573,8 +576,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="417600" y="7200"/>
-          <a:ext cx="1761480" cy="358200"/>
+          <a:off x="444600" y="7200"/>
+          <a:ext cx="1780200" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -589,15 +592,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>520200</xdr:colOff>
+      <xdr:colOff>547200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>5040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1563120</xdr:colOff>
+      <xdr:colOff>1589760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>330120</xdr:rowOff>
+      <xdr:rowOff>329760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -610,8 +613,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2415600" y="5040"/>
-          <a:ext cx="1042920" cy="325080"/>
+          <a:off x="2461680" y="5040"/>
+          <a:ext cx="1042560" cy="324720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -626,13 +629,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>389880</xdr:colOff>
+      <xdr:colOff>416880</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>389880</xdr:colOff>
+      <xdr:colOff>416880</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>371160</xdr:rowOff>
     </xdr:to>
@@ -643,7 +646,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2285280" y="2880"/>
+          <a:off x="2331360" y="2880"/>
           <a:ext cx="0" cy="368280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -678,15 +681,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>444600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>114480</xdr:colOff>
+      <xdr:colOff>141120</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>365400</xdr:rowOff>
+      <xdr:rowOff>365040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -699,8 +702,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="417600" y="7200"/>
-          <a:ext cx="1801800" cy="358200"/>
+          <a:off x="444600" y="7200"/>
+          <a:ext cx="1820520" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -715,15 +718,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>352800</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>5040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1590120</xdr:colOff>
+      <xdr:colOff>1616760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>330120</xdr:rowOff>
+      <xdr:rowOff>329760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -736,8 +739,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2457720" y="5040"/>
-          <a:ext cx="1237320" cy="325080"/>
+          <a:off x="2503800" y="5040"/>
+          <a:ext cx="1236960" cy="324720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -752,13 +755,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>214920</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>214920</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>371160</xdr:rowOff>
     </xdr:to>
@@ -769,7 +772,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2319840" y="2880"/>
+          <a:off x="2365920" y="2880"/>
           <a:ext cx="0" cy="368280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -804,15 +807,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>444600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2181240</xdr:colOff>
+      <xdr:colOff>2207880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>365400</xdr:rowOff>
+      <xdr:rowOff>365040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -825,8 +828,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="417600" y="7200"/>
-          <a:ext cx="1763640" cy="358200"/>
+          <a:off x="444600" y="7200"/>
+          <a:ext cx="1763280" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -841,15 +844,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2411280</xdr:colOff>
+      <xdr:colOff>2438280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>5040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1038960</xdr:colOff>
+      <xdr:colOff>1065600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>330120</xdr:rowOff>
+      <xdr:rowOff>329760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -862,8 +865,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2411280" y="5040"/>
-          <a:ext cx="1332720" cy="325080"/>
+          <a:off x="2438280" y="5040"/>
+          <a:ext cx="1351440" cy="324720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -878,13 +881,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2273400</xdr:colOff>
+      <xdr:colOff>2300400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2273400</xdr:colOff>
+      <xdr:colOff>2300400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>371160</xdr:rowOff>
     </xdr:to>
@@ -895,7 +898,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2273400" y="2880"/>
+          <a:off x="2300400" y="2880"/>
           <a:ext cx="0" cy="368280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -932,16 +935,16 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="111.619433198381"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="112.688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
@@ -1169,11 +1172,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -3812,13 +3815,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -7024,16 +7027,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -7098,6 +7101,14 @@
         <v>44</v>
       </c>
       <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -7125,8 +7136,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -7145,7 +7156,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7621,17 +7632,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7639,7 +7650,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7647,7 +7658,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7655,7 +7666,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7663,7 +7674,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7671,7 +7682,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7679,7 +7690,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7687,7 +7698,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -7715,9 +7726,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7735,21 +7746,21 @@
     </row>
     <row r="3" s="22" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>2</v>
@@ -7763,7 +7774,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>3</v>
@@ -7777,7 +7788,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>5</v>
@@ -7791,7 +7802,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>2</v>
@@ -7805,7 +7816,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>3</v>
@@ -7819,7 +7830,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>5</v>
@@ -7833,7 +7844,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>5</v>
@@ -7847,7 +7858,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>4</v>
@@ -7861,7 +7872,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>5</v>
@@ -7875,7 +7886,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" s="23" t="n">
         <v>6</v>
@@ -7889,7 +7900,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="23" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
copy diageous-sand2 to prod and sand
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS_SAND/Data/Template.xlsx
+++ b/Projects/DIAGEOUS_SAND/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="independent - off_trade" sheetId="1" state="visible" r:id="rId2"/>
@@ -357,14 +357,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0242914979757"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -434,14 +434,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -497,15 +497,15 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -595,20 +595,20 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.1336032388664"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>